<commit_message>
move network, fill in zeros
</commit_message>
<xml_diff>
--- a/Network.xlsx
+++ b/Network.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cortbreuer/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cortbreuer/Desktop/Storage/Cornell/Junior Spring 2021/CHEME 5440/Problem Sets/Problem Set 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6580A8D5-0B9A-FB4C-938B-F3FF5FC1BC49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1CC779-D0C0-8B4B-ABE1-43C0A878A1B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1760" yWindow="1800" windowWidth="27640" windowHeight="16940" xr2:uid="{379B21F9-82EB-AF42-A745-AB6F00DAD8C8}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H3" sqref="H3:Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,57 +575,198 @@
       <c r="H3">
         <v>1</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
       <c r="O3">
         <v>-1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
       <c r="I4">
         <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
       </c>
       <c r="L4">
         <v>-1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
       <c r="J5">
         <v>-1</v>
       </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
       <c r="M5">
         <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
       <c r="K6">
         <v>-1</v>
       </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
       <c r="N6">
         <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
       <c r="L7">
         <v>-1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
       <c r="L8">
         <v>-1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -641,38 +782,134 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
       <c r="L9">
         <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
       <c r="L10">
         <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11">
         <v>-1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
       <c r="M12">
         <v>1</v>
       </c>
       <c r="N12">
         <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
       </c>
       <c r="P12">
         <v>-2</v>
@@ -685,8 +922,29 @@
       <c r="A13" t="s">
         <v>19</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="N13">
         <v>-1</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
       </c>
       <c r="P13">
         <v>2</v>
@@ -699,25 +957,100 @@
       <c r="A14" t="s">
         <v>20</v>
       </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14">
         <v>-1</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
       <c r="O15">
         <v>1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
       <c r="P16">
         <v>-1</v>
       </c>
@@ -729,6 +1062,30 @@
       <c r="A17" t="s">
         <v>23</v>
       </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
       <c r="P17">
         <v>-2</v>
       </c>
@@ -740,6 +1097,30 @@
       <c r="A18" t="s">
         <v>24</v>
       </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
       <c r="P18">
         <v>-1</v>
       </c>
@@ -751,6 +1132,30 @@
       <c r="A19" t="s">
         <v>25</v>
       </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
       <c r="P19">
         <v>1</v>
       </c>
@@ -761,6 +1166,30 @@
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
       </c>
       <c r="P20">
         <v>2</v>

</xml_diff>

<commit_message>
Updates to element balance
</commit_message>
<xml_diff>
--- a/Network.xlsx
+++ b/Network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cortbreuer/Desktop/Storage/Cornell/Junior Spring 2021/CHEME 5440/Problem Sets/Problem Set 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6DD0D8-18C5-FD49-B4BB-6F7CFBD09AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F3E98A-D171-A847-B6D8-43E1E08A6FC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="1800" windowWidth="27640" windowHeight="16940" xr2:uid="{379B21F9-82EB-AF42-A745-AB6F00DAD8C8}"/>
+    <workbookView xWindow="1920" yWindow="3060" windowWidth="27640" windowHeight="16940" xr2:uid="{379B21F9-82EB-AF42-A745-AB6F00DAD8C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>b1</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>-v5</t>
   </si>
   <si>
     <t>Molecular Composition</t>
@@ -214,9 +211,6 @@
   </si>
   <si>
     <t>b19</t>
-  </si>
-  <si>
-    <t>c</t>
   </si>
 </sst>
 </file>
@@ -575,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFC1012-8B2A-0F43-BFCB-3CCC7650DDEE}">
   <dimension ref="A1:AG107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:Z65"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:Y65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,155 +579,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="N2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="O2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="Q2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="R2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="T2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="U2" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="V2" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="W2" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="X2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD2" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AF2" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="Z2" s="1"/>
       <c r="AG2" s="1"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA3">
-        <v>2</v>
-      </c>
-      <c r="AB3">
-        <v>2</v>
-      </c>
-      <c r="AC3">
-        <v>2</v>
-      </c>
-      <c r="AD3">
-        <v>2</v>
-      </c>
-      <c r="AE3" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="Y3" s="1"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -743,22 +697,22 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -806,30 +760,13 @@
         <v>0</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>-1</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
+        <f>SUM(B4:Y4)</f>
         <v>0</v>
       </c>
     </row>
@@ -838,16 +775,16 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -859,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -895,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -910,24 +847,7 @@
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>-1</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
+        <f t="shared" ref="Z5:Z22" si="0">SUM(B5:Y5)</f>
         <v>0</v>
       </c>
     </row>
@@ -936,16 +856,16 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -960,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -996,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -1008,24 +928,7 @@
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>1</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1034,16 +937,16 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1061,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1097,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -1106,24 +1009,7 @@
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <v>1</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <v>0</v>
-      </c>
-      <c r="AF7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1132,19 +1018,19 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1162,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1189,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1204,24 +1090,7 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>-1</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AF8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1230,22 +1099,22 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1263,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1287,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -1296,31 +1165,14 @@
         <v>0</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>-1</v>
-      </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <v>0</v>
-      </c>
-      <c r="AD9">
-        <v>1</v>
-      </c>
-      <c r="AE9">
-        <v>-2</v>
-      </c>
-      <c r="AF9">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
@@ -1328,25 +1180,25 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1364,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1385,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1400,24 +1252,7 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <v>1</v>
-      </c>
-      <c r="AB10">
-        <v>0</v>
-      </c>
-      <c r="AC10">
-        <v>0</v>
-      </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AF10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1429,16 +1264,16 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1447,7 +1282,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1465,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1483,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -1498,24 +1333,7 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>1</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1524,16 +1342,16 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1566,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -1581,10 +1399,10 @@
         <v>0</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1596,24 +1414,7 @@
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AA12">
-        <v>1</v>
-      </c>
-      <c r="AB12">
-        <v>-1</v>
-      </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
-      <c r="AF12">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1622,16 +1423,16 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1667,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -1682,10 +1483,10 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -1694,42 +1495,25 @@
         <v>0</v>
       </c>
       <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
-      <c r="AB13">
-        <v>1</v>
-      </c>
-      <c r="AC13">
-        <v>-1</v>
-      </c>
-      <c r="AD13">
-        <v>0</v>
-      </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
-      <c r="AF13">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1750,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1768,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -1789,28 +1573,11 @@
         <v>0</v>
       </c>
       <c r="Y14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
-      <c r="AB14">
-        <v>0</v>
-      </c>
-      <c r="AC14">
-        <v>0</v>
-      </c>
-      <c r="AD14">
-        <v>0</v>
-      </c>
-      <c r="AE14">
-        <v>2</v>
-      </c>
-      <c r="AF14">
-        <v>-2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.2">
@@ -1821,13 +1588,13 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1851,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -1869,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <v>0</v>
@@ -1881,34 +1648,17 @@
         <v>0</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X15">
         <v>0</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
-      <c r="AC15">
-        <v>-1</v>
-      </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
-      <c r="AE15">
-        <v>-2</v>
-      </c>
-      <c r="AF15">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.2">
@@ -1916,16 +1666,16 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1970,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16">
         <v>0</v>
@@ -1979,33 +1729,16 @@
         <v>0</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y16">
         <v>0</v>
       </c>
       <c r="Z16">
-        <v>0</v>
-      </c>
-      <c r="AA16">
-        <v>0</v>
-      </c>
-      <c r="AB16">
-        <v>0</v>
-      </c>
-      <c r="AC16">
-        <v>1</v>
-      </c>
-      <c r="AD16">
-        <v>-1</v>
-      </c>
-      <c r="AE16">
-        <v>0</v>
-      </c>
-      <c r="AF16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2017,16 +1750,16 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2053,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -2071,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="U17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -2080,30 +1813,13 @@
         <v>0</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y17">
         <v>0</v>
       </c>
       <c r="Z17">
-        <v>0</v>
-      </c>
-      <c r="AA17">
-        <v>0</v>
-      </c>
-      <c r="AB17">
-        <v>0</v>
-      </c>
-      <c r="AC17">
-        <v>0</v>
-      </c>
-      <c r="AD17">
-        <v>1</v>
-      </c>
-      <c r="AE17">
-        <v>0</v>
-      </c>
-      <c r="AF17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2112,19 +1828,19 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2154,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -2172,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="V18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -2181,28 +1897,11 @@
         <v>0</v>
       </c>
       <c r="Y18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AA18">
-        <v>0</v>
-      </c>
-      <c r="AB18">
-        <v>0</v>
-      </c>
-      <c r="AC18">
-        <v>0</v>
-      </c>
-      <c r="AD18">
-        <v>0</v>
-      </c>
-      <c r="AE18">
-        <v>1</v>
-      </c>
-      <c r="AF18">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
@@ -2219,88 +1918,71 @@
         <v>0</v>
       </c>
       <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>-2</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
         <v>2</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19">
-        <v>1</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
       <c r="Z19">
-        <v>0</v>
-      </c>
-      <c r="AA19">
-        <v>0</v>
-      </c>
-      <c r="AB19">
-        <v>0</v>
-      </c>
-      <c r="AC19">
-        <v>0</v>
-      </c>
-      <c r="AD19">
-        <v>0</v>
-      </c>
-      <c r="AE19">
-        <v>2</v>
-      </c>
-      <c r="AF19">
-        <v>-2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
@@ -2311,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2356,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S20">
         <v>0</v>
@@ -2374,31 +2056,14 @@
         <v>0</v>
       </c>
       <c r="X20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z20">
-        <v>0</v>
-      </c>
-      <c r="AA20">
-        <v>0</v>
-      </c>
-      <c r="AB20">
-        <v>0</v>
-      </c>
-      <c r="AC20">
-        <v>0</v>
-      </c>
-      <c r="AD20">
-        <v>0</v>
-      </c>
-      <c r="AE20">
-        <v>1</v>
-      </c>
-      <c r="AF20">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
@@ -2406,19 +2071,19 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2457,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21">
         <v>0</v>
@@ -2475,28 +2140,11 @@
         <v>0</v>
       </c>
       <c r="Y21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AA21">
-        <v>0</v>
-      </c>
-      <c r="AB21">
-        <v>0</v>
-      </c>
-      <c r="AC21">
-        <v>0</v>
-      </c>
-      <c r="AD21">
-        <v>0</v>
-      </c>
-      <c r="AE21">
-        <v>-1</v>
-      </c>
-      <c r="AF21">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
@@ -2510,10 +2158,10 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -2558,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -2573,33 +2221,16 @@
         <v>0</v>
       </c>
       <c r="Y22">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Z22">
-        <v>1</v>
-      </c>
-      <c r="AA22">
-        <v>0</v>
-      </c>
-      <c r="AB22">
-        <v>0</v>
-      </c>
-      <c r="AC22">
-        <v>0</v>
-      </c>
-      <c r="AD22">
-        <v>0</v>
-      </c>
-      <c r="AE22">
-        <v>-2</v>
-      </c>
-      <c r="AF22">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2634,22 +2265,22 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" t="s">
         <v>30</v>
       </c>
-      <c r="C24" t="s">
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" t="s">
         <v>48</v>
-      </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" t="s">
-        <v>49</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
@@ -2667,58 +2298,58 @@
         <v>8</v>
       </c>
       <c r="M24" t="s">
+        <v>52</v>
+      </c>
+      <c r="N24" t="s">
         <v>53</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>54</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>55</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>56</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
+        <v>29</v>
+      </c>
+      <c r="S24" t="s">
+        <v>47</v>
+      </c>
+      <c r="T24" t="s">
+        <v>31</v>
+      </c>
+      <c r="U24" t="s">
+        <v>30</v>
+      </c>
+      <c r="V24" t="s">
+        <v>32</v>
+      </c>
+      <c r="W24" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y24" t="s">
         <v>57</v>
       </c>
-      <c r="R24" t="s">
+      <c r="Z24" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC24" t="s">
         <v>30</v>
       </c>
-      <c r="S24" t="s">
+      <c r="AD24" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE24" t="s">
         <v>48</v>
-      </c>
-      <c r="T24" t="s">
-        <v>32</v>
-      </c>
-      <c r="U24" t="s">
-        <v>31</v>
-      </c>
-      <c r="V24" t="s">
-        <v>33</v>
-      </c>
-      <c r="W24" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.2">
@@ -2763,70 +2394,70 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25:P40" si="0">2*I25</f>
+        <f t="shared" ref="N25:P40" si="1">2*I25</f>
         <v>0</v>
       </c>
       <c r="O25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="Q25">
         <v>0</v>
       </c>
       <c r="R25">
-        <f>B25*($M25+$N25+$O25+$P25+$Q25)</f>
+        <f t="shared" ref="R25:W25" si="2">B25*($M25+$N25+$O25+$P25+$Q25)</f>
         <v>-2</v>
       </c>
       <c r="S25">
-        <f>C25*($M25+$N25+$O25+$P25+$Q25)</f>
+        <f t="shared" si="2"/>
         <v>-8</v>
       </c>
       <c r="T25">
-        <f>D25*($M25+$N25+$O25+$P25+$Q25)</f>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="U25">
-        <f>E25*($M25+$N25+$O25+$P25+$Q25)</f>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="V25">
-        <f>F25*($M25+$N25+$O25+$P25+$Q25)</f>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="W25">
-        <f>G25*($M25+$N25+$O25+$P25+$Q25)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y25">
-        <f>SUM(M25:Q25)</f>
+        <f t="shared" ref="Y25:Y43" si="3">SUM(M25:Q25)</f>
         <v>-2</v>
       </c>
       <c r="Z25">
-        <f>$Y25*B25</f>
+        <f t="shared" ref="Z25:Z43" si="4">$Y25*B25</f>
         <v>-2</v>
       </c>
       <c r="AA25">
-        <f>$Y25*C25</f>
+        <f t="shared" ref="AA25:AA43" si="5">$Y25*C25</f>
         <v>-8</v>
       </c>
       <c r="AB25">
-        <f>$Y25*D25</f>
+        <f t="shared" ref="AB25:AB43" si="6">$Y25*D25</f>
         <v>-2</v>
       </c>
       <c r="AC25">
-        <f>$Y25*E25</f>
+        <f t="shared" ref="AC25:AC43" si="7">$Y25*E25</f>
         <v>-10</v>
       </c>
       <c r="AD25">
-        <f>$Y25*F25</f>
+        <f t="shared" ref="AD25:AD43" si="8">$Y25*F25</f>
         <v>-2</v>
       </c>
       <c r="AE25">
-        <f>$Y25*G25</f>
+        <f t="shared" ref="AE25:AE43" si="9">$Y25*G25</f>
         <v>0</v>
       </c>
     </row>
@@ -2868,74 +2499,74 @@
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26:M43" si="1">2*H26</f>
+        <f t="shared" ref="M26:M43" si="10">2*H26</f>
         <v>-2</v>
       </c>
       <c r="N26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q26">
         <v>0</v>
       </c>
       <c r="R26">
-        <f t="shared" ref="R26:U43" si="2">B26*($M26+$N26+$O26+$P26+$Q26)</f>
+        <f t="shared" ref="R26:U43" si="11">B26*($M26+$N26+$O26+$P26+$Q26)</f>
         <v>-8</v>
       </c>
       <c r="S26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-14</v>
       </c>
       <c r="T26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-2</v>
       </c>
       <c r="U26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-8</v>
       </c>
       <c r="V26">
-        <f t="shared" ref="V26:V43" si="3">F26*($M26+$N26+$O26+$P26+$Q26)</f>
+        <f t="shared" ref="V26:V43" si="12">F26*($M26+$N26+$O26+$P26+$Q26)</f>
         <v>0</v>
       </c>
       <c r="W26">
-        <f t="shared" ref="W26:W43" si="4">G26*($M26+$N26+$O26+$P26+$Q26)</f>
+        <f t="shared" ref="W26:W43" si="13">G26*($M26+$N26+$O26+$P26+$Q26)</f>
         <v>0</v>
       </c>
       <c r="Y26">
-        <f>SUM(M26:Q26)</f>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
       <c r="Z26">
-        <f>$Y26*B26</f>
+        <f t="shared" si="4"/>
         <v>-8</v>
       </c>
       <c r="AA26">
-        <f>$Y26*C26</f>
+        <f t="shared" si="5"/>
         <v>-14</v>
       </c>
       <c r="AB26">
-        <f>$Y26*D26</f>
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
       <c r="AC26">
-        <f>$Y26*E26</f>
+        <f t="shared" si="7"/>
         <v>-8</v>
       </c>
       <c r="AD26">
-        <f>$Y26*F26</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE26">
-        <f>$Y26*G26</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2977,74 +2608,74 @@
         <v>0</v>
       </c>
       <c r="M27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="O27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q27">
         <v>0</v>
       </c>
       <c r="R27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="S27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="T27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="V27">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y27">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W27">
+        <v>2</v>
+      </c>
+      <c r="Z27">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y27">
-        <f>SUM(M27:Q27)</f>
-        <v>2</v>
-      </c>
-      <c r="Z27">
-        <f>$Y27*B27</f>
         <v>8</v>
       </c>
       <c r="AA27">
-        <f>$Y27*C27</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="AB27">
-        <f>$Y27*D27</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC27">
-        <f>$Y27*E27</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="AD27">
-        <f>$Y27*F27</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE27">
-        <f>$Y27*G27</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3086,74 +2717,74 @@
         <v>0</v>
       </c>
       <c r="M28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="O28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q28">
         <v>0</v>
       </c>
       <c r="R28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="S28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="T28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="U28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="V28">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y28">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W28">
+        <v>2</v>
+      </c>
+      <c r="Z28">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y28">
-        <f>SUM(M28:Q28)</f>
         <v>2</v>
       </c>
-      <c r="Z28">
-        <f>$Y28*B28</f>
+      <c r="AA28">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AB28">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="AA28">
-        <f>$Y28*C28</f>
-        <v>8</v>
-      </c>
-      <c r="AB28">
-        <f>$Y28*D28</f>
-        <v>4</v>
-      </c>
-      <c r="AC28">
-        <f>$Y28*E28</f>
-        <v>2</v>
-      </c>
       <c r="AD28">
-        <f>$Y28*F28</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE28">
-        <f>$Y28*G28</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3195,74 +2826,74 @@
         <v>0</v>
       </c>
       <c r="M29">
+        <f t="shared" si="10"/>
+        <v>-2</v>
+      </c>
+      <c r="N29">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="11"/>
+        <v>-20</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="11"/>
+        <v>-32</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="11"/>
+        <v>-10</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="11"/>
+        <v>-26</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="12"/>
+        <v>-6</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
-      <c r="N29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="2"/>
+      <c r="Z29">
+        <f t="shared" si="4"/>
         <v>-20</v>
       </c>
-      <c r="S29">
-        <f t="shared" si="2"/>
+      <c r="AA29">
+        <f t="shared" si="5"/>
         <v>-32</v>
       </c>
-      <c r="T29">
-        <f t="shared" si="2"/>
+      <c r="AB29">
+        <f t="shared" si="6"/>
         <v>-10</v>
       </c>
-      <c r="U29">
-        <f t="shared" si="2"/>
+      <c r="AC29">
+        <f t="shared" si="7"/>
         <v>-26</v>
       </c>
-      <c r="V29">
-        <f t="shared" si="3"/>
+      <c r="AD29">
+        <f t="shared" si="8"/>
         <v>-6</v>
       </c>
-      <c r="W29">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y29">
-        <f>SUM(M29:Q29)</f>
-        <v>-2</v>
-      </c>
-      <c r="Z29">
-        <f>$Y29*B29</f>
-        <v>-20</v>
-      </c>
-      <c r="AA29">
-        <f>$Y29*C29</f>
-        <v>-32</v>
-      </c>
-      <c r="AB29">
-        <f>$Y29*D29</f>
-        <v>-10</v>
-      </c>
-      <c r="AC29">
-        <f>$Y29*E29</f>
-        <v>-26</v>
-      </c>
-      <c r="AD29">
-        <f>$Y29*F29</f>
-        <v>-6</v>
-      </c>
       <c r="AE29">
-        <f>$Y29*G29</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3304,74 +2935,74 @@
         <v>-2</v>
       </c>
       <c r="M30">
+        <f t="shared" si="10"/>
+        <v>-2</v>
+      </c>
+      <c r="N30">
         <f t="shared" si="1"/>
-        <v>-2</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q30">
         <v>-2</v>
       </c>
       <c r="R30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-12</v>
       </c>
       <c r="S30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-26</v>
       </c>
       <c r="T30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-6</v>
       </c>
       <c r="U30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-6</v>
       </c>
       <c r="V30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y30">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W30">
+        <v>-2</v>
+      </c>
+      <c r="Z30">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y30">
-        <f>SUM(M30:Q30)</f>
-        <v>-2</v>
-      </c>
-      <c r="Z30">
-        <f>$Y30*B30</f>
         <v>-12</v>
       </c>
       <c r="AA30">
-        <f>$Y30*C30</f>
+        <f t="shared" si="5"/>
         <v>-26</v>
       </c>
       <c r="AB30">
-        <f>$Y30*D30</f>
+        <f t="shared" si="6"/>
         <v>-6</v>
       </c>
       <c r="AC30">
-        <f>$Y30*E30</f>
+        <f t="shared" si="7"/>
         <v>-6</v>
       </c>
       <c r="AD30">
-        <f>$Y30*F30</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE30">
-        <f>$Y30*G30</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3413,74 +3044,74 @@
         <v>0</v>
       </c>
       <c r="M31">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="N31">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="11"/>
+        <v>28</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
-      <c r="N31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="V31">
+      <c r="W31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y31">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="W31">
+      <c r="Z31">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y31">
-        <f>SUM(M31:Q31)</f>
+        <v>20</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="Z31">
-        <f>$Y31*B31</f>
-        <v>20</v>
-      </c>
-      <c r="AA31">
-        <f>$Y31*C31</f>
-        <v>28</v>
-      </c>
-      <c r="AB31">
-        <f>$Y31*D31</f>
-        <v>10</v>
-      </c>
-      <c r="AC31">
-        <f>$Y31*E31</f>
-        <v>14</v>
-      </c>
-      <c r="AD31">
-        <f>$Y31*F31</f>
-        <v>2</v>
-      </c>
       <c r="AE31">
-        <f>$Y31*G31</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3522,74 +3153,74 @@
         <v>0</v>
       </c>
       <c r="M32">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="N32">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="N32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="2"/>
+      <c r="Z32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="T32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U32">
-        <f t="shared" si="2"/>
+      <c r="AB32">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC32">
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="V32">
-        <f t="shared" si="3"/>
+      <c r="AD32">
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="W32">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y32">
-        <f>SUM(M32:Q32)</f>
-        <v>2</v>
-      </c>
-      <c r="Z32">
-        <f>$Y32*B32</f>
-        <v>0</v>
-      </c>
-      <c r="AA32">
-        <f>$Y32*C32</f>
-        <v>8</v>
-      </c>
-      <c r="AB32">
-        <f>$Y32*D32</f>
-        <v>0</v>
-      </c>
-      <c r="AC32">
-        <f>$Y32*E32</f>
-        <v>14</v>
-      </c>
-      <c r="AD32">
-        <f>$Y32*F32</f>
-        <v>4</v>
-      </c>
       <c r="AE32">
-        <f>$Y32*G32</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3631,74 +3262,74 @@
         <v>0</v>
       </c>
       <c r="M33">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="N33">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="O33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q33">
         <v>0</v>
       </c>
       <c r="R33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V33">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W33">
+      <c r="Z33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y33">
-        <f>SUM(M33:Q33)</f>
-        <v>0</v>
-      </c>
-      <c r="Z33">
-        <f>$Y33*B33</f>
-        <v>0</v>
-      </c>
       <c r="AA33">
-        <f>$Y33*C33</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB33">
-        <f>$Y33*D33</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC33">
-        <f>$Y33*E33</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD33">
-        <f>$Y33*F33</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE33">
-        <f>$Y33*G33</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3740,80 +3371,80 @@
         <v>0</v>
       </c>
       <c r="M34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N34">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="O34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="P34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q34">
         <v>0</v>
       </c>
       <c r="R34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V34">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y34">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W34">
+      <c r="Z34">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y34">
-        <f>SUM(M34:Q34)</f>
-        <v>0</v>
-      </c>
-      <c r="Z34">
-        <f>$Y34*B34</f>
-        <v>0</v>
-      </c>
       <c r="AA34">
-        <f>$Y34*C34</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB34">
-        <f>$Y34*D34</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC34">
-        <f>$Y34*E34</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD34">
-        <f>$Y34*F34</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE34">
-        <f>$Y34*G34</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35">
         <v>6</v>
@@ -3849,74 +3480,74 @@
         <v>2</v>
       </c>
       <c r="M35">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="O35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q35">
         <v>2</v>
       </c>
       <c r="R35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="S35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>28</v>
       </c>
       <c r="T35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="U35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="V35">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y35">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W35">
+        <v>2</v>
+      </c>
+      <c r="Z35">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y35">
-        <f>SUM(M35:Q35)</f>
-        <v>2</v>
-      </c>
-      <c r="Z35">
-        <f>$Y35*B35</f>
         <v>12</v>
       </c>
       <c r="AA35">
-        <f>$Y35*C35</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="AB35">
-        <f>$Y35*D35</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="AC35">
-        <f>$Y35*E35</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="AD35">
-        <f>$Y35*F35</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE35">
-        <f>$Y35*G35</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3958,74 +3589,74 @@
         <v>-2</v>
       </c>
       <c r="M36">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="O36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="P36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q36">
         <v>-2</v>
       </c>
       <c r="R36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-8</v>
       </c>
       <c r="T36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-4</v>
       </c>
       <c r="V36">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y36">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W36">
+        <v>-4</v>
+      </c>
+      <c r="Z36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y36">
-        <f>SUM(M36:Q36)</f>
+      <c r="AA36">
+        <f t="shared" si="5"/>
+        <v>-8</v>
+      </c>
+      <c r="AB36">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <f t="shared" si="7"/>
         <v>-4</v>
       </c>
-      <c r="Z36">
-        <f>$Y36*B36</f>
-        <v>0</v>
-      </c>
-      <c r="AA36">
-        <f>$Y36*C36</f>
-        <v>-8</v>
-      </c>
-      <c r="AB36">
-        <f>$Y36*D36</f>
-        <v>0</v>
-      </c>
-      <c r="AC36">
-        <f>$Y36*E36</f>
-        <v>-4</v>
-      </c>
       <c r="AD36">
-        <f>$Y36*F36</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE36">
-        <f>$Y36*G36</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4067,74 +3698,74 @@
         <v>0</v>
       </c>
       <c r="M37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="O37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="Q37">
         <v>0</v>
       </c>
       <c r="R37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V37">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y37">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W37">
+      <c r="Z37">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y37">
-        <f>SUM(M37:Q37)</f>
-        <v>0</v>
-      </c>
-      <c r="Z37">
-        <f>$Y37*B37</f>
-        <v>0</v>
-      </c>
       <c r="AA37">
-        <f>$Y37*C37</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB37">
-        <f>$Y37*D37</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC37">
-        <f>$Y37*E37</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD37">
-        <f>$Y37*F37</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE37">
-        <f>$Y37*G37</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4176,74 +3807,74 @@
         <v>0</v>
       </c>
       <c r="M38">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="O38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q38">
         <v>0</v>
       </c>
       <c r="R38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="T38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="V38">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y38">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="W38">
+      <c r="Z38">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y38">
-        <f>SUM(M38:Q38)</f>
+      <c r="AA38">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="Z38">
-        <f>$Y38*B38</f>
-        <v>0</v>
-      </c>
-      <c r="AA38">
-        <f>$Y38*C38</f>
-        <v>6</v>
-      </c>
-      <c r="AB38">
-        <f>$Y38*D38</f>
-        <v>0</v>
-      </c>
-      <c r="AC38">
-        <f>$Y38*E38</f>
-        <v>8</v>
-      </c>
-      <c r="AD38">
-        <f>$Y38*F38</f>
-        <v>2</v>
-      </c>
       <c r="AE38">
-        <f>$Y38*G38</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4285,74 +3916,74 @@
         <v>1</v>
       </c>
       <c r="M39">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="O39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q39">
         <v>1</v>
       </c>
       <c r="R39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
       <c r="S39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>30</v>
       </c>
       <c r="T39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="U39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>17</v>
       </c>
       <c r="V39">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y39">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="AB39">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="AC39">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="AD39">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="W39">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y39">
-        <f>SUM(M39:Q39)</f>
-        <v>1</v>
-      </c>
-      <c r="Z39">
-        <f>$Y39*B39</f>
-        <v>21</v>
-      </c>
-      <c r="AA39">
-        <f>$Y39*C39</f>
-        <v>30</v>
-      </c>
-      <c r="AB39">
-        <f>$Y39*D39</f>
-        <v>7</v>
-      </c>
-      <c r="AC39">
-        <f>$Y39*E39</f>
-        <v>17</v>
-      </c>
-      <c r="AD39">
-        <f>$Y39*F39</f>
-        <v>3</v>
-      </c>
       <c r="AE39">
-        <f>$Y39*G39</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4394,74 +4025,74 @@
         <v>2</v>
       </c>
       <c r="M40">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="O40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q40">
         <v>2</v>
       </c>
       <c r="R40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="V40">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y40">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W40">
+        <v>2</v>
+      </c>
+      <c r="Z40">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y40">
-        <f>SUM(M40:Q40)</f>
-        <v>2</v>
-      </c>
-      <c r="Z40">
-        <f>$Y40*B40</f>
-        <v>0</v>
-      </c>
       <c r="AA40">
-        <f>$Y40*C40</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB40">
-        <f>$Y40*D40</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC40">
-        <f>$Y40*E40</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="AD40">
-        <f>$Y40*F40</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE40">
-        <f>$Y40*G40</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4503,74 +4134,74 @@
         <v>1</v>
       </c>
       <c r="M41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N41">
-        <f t="shared" ref="N41:N43" si="5">2*I41</f>
+        <f t="shared" ref="N41:N43" si="14">2*I41</f>
         <v>0</v>
       </c>
       <c r="O41">
-        <f t="shared" ref="O41:O43" si="6">2*J41</f>
+        <f t="shared" ref="O41:O43" si="15">2*J41</f>
         <v>0</v>
       </c>
       <c r="P41">
-        <f t="shared" ref="P41:P43" si="7">2*K41</f>
+        <f t="shared" ref="P41:P43" si="16">2*K41</f>
         <v>0</v>
       </c>
       <c r="Q41">
         <v>1</v>
       </c>
       <c r="R41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="T41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V41">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y41">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="Z41">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y41">
-        <f>SUM(M41:Q41)</f>
-        <v>1</v>
-      </c>
-      <c r="Z41">
-        <f>$Y41*B41</f>
-        <v>0</v>
-      </c>
       <c r="AA41">
-        <f>$Y41*C41</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AB41">
-        <f>$Y41*D41</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC41">
-        <f>$Y41*E41</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD41">
-        <f>$Y41*F41</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE41">
-        <f>$Y41*G41</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4612,74 +4243,74 @@
         <v>-1</v>
       </c>
       <c r="M42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q42">
         <v>-1</v>
       </c>
       <c r="R42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-21</v>
       </c>
       <c r="S42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-29</v>
       </c>
       <c r="T42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-7</v>
       </c>
       <c r="U42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-17</v>
       </c>
       <c r="V42">
+        <f t="shared" si="12"/>
+        <v>-3</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y42">
         <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="4"/>
+        <v>-21</v>
+      </c>
+      <c r="AA42">
+        <f t="shared" si="5"/>
+        <v>-29</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="6"/>
+        <v>-7</v>
+      </c>
+      <c r="AC42">
+        <f t="shared" si="7"/>
+        <v>-17</v>
+      </c>
+      <c r="AD42">
+        <f t="shared" si="8"/>
         <v>-3</v>
       </c>
-      <c r="W42">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y42">
-        <f>SUM(M42:Q42)</f>
-        <v>-1</v>
-      </c>
-      <c r="Z42">
-        <f>$Y42*B42</f>
-        <v>-21</v>
-      </c>
-      <c r="AA42">
-        <f>$Y42*C42</f>
-        <v>-29</v>
-      </c>
-      <c r="AB42">
-        <f>$Y42*D42</f>
-        <v>-7</v>
-      </c>
-      <c r="AC42">
-        <f>$Y42*E42</f>
-        <v>-17</v>
-      </c>
-      <c r="AD42">
-        <f>$Y42*F42</f>
-        <v>-3</v>
-      </c>
       <c r="AE42">
-        <f>$Y42*G42</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -4721,95 +4352,95 @@
         <v>-2</v>
       </c>
       <c r="M43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="Q43">
         <v>-2</v>
       </c>
       <c r="R43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="T43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-2</v>
       </c>
       <c r="U43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>-2</v>
       </c>
       <c r="V43">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y43">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W43">
+        <v>-2</v>
+      </c>
+      <c r="Z43">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y43">
-        <f>SUM(M43:Q43)</f>
+      <c r="AA43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB43">
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
-      <c r="Z43">
-        <f>$Y43*B43</f>
-        <v>0</v>
-      </c>
-      <c r="AA43">
-        <f>$Y43*C43</f>
-        <v>0</v>
-      </c>
-      <c r="AB43">
-        <f>$Y43*D43</f>
+      <c r="AC43">
+        <f t="shared" si="7"/>
         <v>-2</v>
       </c>
-      <c r="AC43">
-        <f>$Y43*E43</f>
-        <v>-2</v>
-      </c>
       <c r="AD43">
-        <f>$Y43*F43</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE43">
-        <f>$Y43*G43</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R44">
         <f>SUM(R25:R43)</f>
         <v>0</v>
       </c>
       <c r="S44">
-        <f t="shared" ref="R44:U44" si="8">SUM(S25:S43)</f>
+        <f t="shared" ref="S44:U44" si="17">SUM(S25:S43)</f>
         <v>0</v>
       </c>
       <c r="T44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="V44">
@@ -4825,29 +4456,29 @@
         <v>0</v>
       </c>
       <c r="AA44">
-        <f t="shared" ref="AA44:AE44" si="9">SUM(AA25:AA43)</f>
+        <f t="shared" ref="AA44:AE44" si="18">SUM(AA25:AA43)</f>
         <v>0</v>
       </c>
       <c r="AB44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AC44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AD44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AE44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>60</v>
+      <c r="B47">
+        <v>1</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -4913,7 +4544,7 @@
         <v>0</v>
       </c>
       <c r="X47">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="Y47">
         <v>0</v>
@@ -4981,7 +4612,7 @@
         <v>0</v>
       </c>
       <c r="U48">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="V48">
         <v>0</v>
@@ -5061,7 +4692,7 @@
         <v>0</v>
       </c>
       <c r="V49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W49">
         <v>0</v>
@@ -5141,7 +4772,7 @@
         <v>0</v>
       </c>
       <c r="W50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X50">
         <v>0</v>
@@ -5212,7 +4843,7 @@
         <v>0</v>
       </c>
       <c r="U51">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="V51">
         <v>0</v>
@@ -5247,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -5289,7 +4920,7 @@
         <v>0</v>
       </c>
       <c r="U52">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="V52">
         <v>0</v>
@@ -5298,7 +4929,7 @@
         <v>0</v>
       </c>
       <c r="X52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y52">
         <v>-2</v>
@@ -5327,7 +4958,7 @@
         <v>0</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -5366,7 +4997,7 @@
         <v>0</v>
       </c>
       <c r="U53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V53">
         <v>0</v>
@@ -5407,7 +5038,7 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J54">
         <v>0</v>
@@ -5443,7 +5074,7 @@
         <v>0</v>
       </c>
       <c r="U54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V54">
         <v>0</v>
@@ -5487,7 +5118,7 @@
         <v>0</v>
       </c>
       <c r="J55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -5520,10 +5151,10 @@
         <v>0</v>
       </c>
       <c r="U55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V55">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="W55">
         <v>0</v>
@@ -5567,7 +5198,7 @@
         <v>0</v>
       </c>
       <c r="K56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -5600,10 +5231,10 @@
         <v>0</v>
       </c>
       <c r="V56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W56">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="X56">
         <v>0</v>
@@ -5647,7 +5278,7 @@
         <v>0</v>
       </c>
       <c r="L57">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="M57">
         <v>0</v>
@@ -5727,7 +5358,7 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N58">
         <v>0</v>
@@ -5757,7 +5388,7 @@
         <v>0</v>
       </c>
       <c r="W58">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="X58">
         <v>0</v>
@@ -5807,7 +5438,7 @@
         <v>0</v>
       </c>
       <c r="N59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O59">
         <v>0</v>
@@ -5834,10 +5465,10 @@
         <v>0</v>
       </c>
       <c r="W59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X59">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="Y59">
         <v>0</v>
@@ -5887,7 +5518,7 @@
         <v>0</v>
       </c>
       <c r="O60">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="P60">
         <v>0</v>
@@ -5914,7 +5545,7 @@
         <v>0</v>
       </c>
       <c r="X60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y60">
         <v>0</v>
@@ -5967,7 +5598,7 @@
         <v>0</v>
       </c>
       <c r="P61">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Q61">
         <v>0</v>
@@ -6047,7 +5678,7 @@
         <v>0</v>
       </c>
       <c r="Q62">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="R62">
         <v>0</v>
@@ -6127,7 +5758,7 @@
         <v>0</v>
       </c>
       <c r="R63">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S63">
         <v>0</v>
@@ -6287,7 +5918,7 @@
         <v>0</v>
       </c>
       <c r="T65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U65">
         <v>0</v>
@@ -6311,9 +5942,7 @@
     <row r="106" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="107" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:AF1"/>
+  <mergeCells count="1">
     <mergeCell ref="B23:G23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>